<commit_message>
add figure y axies
</commit_message>
<xml_diff>
--- a/simulation/one-taxi/output/100次训练结果比较/司机收入cdf.xlsx
+++ b/simulation/one-taxi/output/100次训练结果比较/司机收入cdf.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC4F9E0-4B05-463C-8C2A-12AA14AA5F7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4071E4BF-D23B-4434-B07E-ABB03A11F170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="510" windowWidth="23625" windowHeight="13065" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2386,11 +2387,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN">
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>CDF </a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>CDF of Income</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4473,10 +4471,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Income(CNY)</a:t>
                 </a:r>
               </a:p>
@@ -4540,9 +4535,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="zh-CN"/>
@@ -4556,6 +4551,7 @@
         <c:axId val="399508287"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4573,6 +4569,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4624,6 +4676,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.81874397835102009"/>
+          <c:y val="0.3579858086680956"/>
+          <c:w val="0.13668046344540985"/>
+          <c:h val="0.223714485775903"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4677,7 +4739,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="zh-CN"/>
     </a:p>
@@ -10008,7 +10073,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>614362</xdr:colOff>
+      <xdr:colOff>515471</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -11873,7 +11938,7 @@
   <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16217,7 +16282,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="C2:C104">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C104">
     <sortCondition ref="C1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -16725,7 +16790,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="L2:L11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:L11">
     <sortCondition ref="L2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>